<commit_message>
dieu chinh mau import hoadon
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
+++ b/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trung Kien\01.Hoa don Bach Khoa\04.Hoa don - Phien ban 2021\Mau nhap khau tu Excel - LK 2021-08-12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\Template\ImportHoaDon\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4921FE-9DA6-4EB4-943C-A6EA7D5124B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9120"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hóa đơn bán hàng" sheetId="1" r:id="rId1"/>
     <sheet name="Nguyên tắc ghép dữ liệu" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="171">
   <si>
     <t>Số thứ tự hóa đơn (*)</t>
   </si>
@@ -151,132 +152,6 @@
   </si>
   <si>
     <t>Tên ngân hàng</t>
-  </si>
-  <si>
-    <t>NM 1</t>
-  </si>
-  <si>
-    <t>NM 2</t>
-  </si>
-  <si>
-    <t>NM 3</t>
-  </si>
-  <si>
-    <t>NM 4</t>
-  </si>
-  <si>
-    <t>NM 5</t>
-  </si>
-  <si>
-    <t>NM 6</t>
-  </si>
-  <si>
-    <t>NM 7</t>
-  </si>
-  <si>
-    <t>NM 8</t>
-  </si>
-  <si>
-    <t>NM 9</t>
-  </si>
-  <si>
-    <t>HHDV 2</t>
-  </si>
-  <si>
-    <t>HHDV 3</t>
-  </si>
-  <si>
-    <t>HHDV 4</t>
-  </si>
-  <si>
-    <t>HHDV 5</t>
-  </si>
-  <si>
-    <t>HHDV 6</t>
-  </si>
-  <si>
-    <t>HHDV 7</t>
-  </si>
-  <si>
-    <t>HHDV 8</t>
-  </si>
-  <si>
-    <t>HHDV 9</t>
-  </si>
-  <si>
-    <t>HHDV 10</t>
-  </si>
-  <si>
-    <t>HHDV 11</t>
-  </si>
-  <si>
-    <t>HHDV 12</t>
-  </si>
-  <si>
-    <t>HHDV 13</t>
-  </si>
-  <si>
-    <t>HHDV 14</t>
-  </si>
-  <si>
-    <t>HHDV 15</t>
-  </si>
-  <si>
-    <t>HHDV 16</t>
-  </si>
-  <si>
-    <t>HHDV 17</t>
-  </si>
-  <si>
-    <t>HHDV 18</t>
-  </si>
-  <si>
-    <t>HHDV 19</t>
-  </si>
-  <si>
-    <t>HHDV 20</t>
-  </si>
-  <si>
-    <t>HHDV 21</t>
-  </si>
-  <si>
-    <t>HHDV 22</t>
-  </si>
-  <si>
-    <t>HHDV 23</t>
-  </si>
-  <si>
-    <t>HHDV 24</t>
-  </si>
-  <si>
-    <t>HHDV 25</t>
-  </si>
-  <si>
-    <t>HHDV 26</t>
-  </si>
-  <si>
-    <t>HHDV 27</t>
-  </si>
-  <si>
-    <t>HHDV 28</t>
-  </si>
-  <si>
-    <t>HHDV 29</t>
-  </si>
-  <si>
-    <t>HHDV 30</t>
-  </si>
-  <si>
-    <t>HHDV 31</t>
-  </si>
-  <si>
-    <t>HHDV 32</t>
-  </si>
-  <si>
-    <t>HHDV 33</t>
-  </si>
-  <si>
-    <t>HHDV 34</t>
   </si>
   <si>
     <t>Thông tin tiền tệ</t>
@@ -413,26 +288,9 @@
     <t>NVBANHANG</t>
   </si>
   <si>
-    <t>DONGCHIETKHAU</t>
-  </si>
-  <si>
-    <t>DONGDIENGIAI</t>
-  </si>
-  <si>
-    <t>Nhập 0 hoặc để trống nếu không là dòng chiết khấu
-Nhâp 1 nếu là dòng chiết khấu</t>
-  </si>
-  <si>
-    <t>Nhập 0 hoặc để trống nếu không là dòng diễn giải, mô tả
-Nhâp 1 nếu là dòng diễn giải, mô tả</t>
-  </si>
-  <si>
     <t xml:space="preserve">- Người dùng muốn nhập thêm thông tin khác: </t>
   </si>
   <si>
-    <t>NM 10</t>
-  </si>
-  <si>
     <t>Mã khách hàng</t>
   </si>
   <si>
@@ -440,12 +298,6 @@
   </si>
   <si>
     <t>- Khai báo dữ liệu hóa đơn cần lập trên Hóa đơn Bách Khoa tại các cột tương ứng trên file này</t>
-  </si>
-  <si>
-    <t>Là dòng chiết khấu</t>
-  </si>
-  <si>
-    <t>Là dòng diễn giải, mô tả</t>
   </si>
   <si>
     <t>Ví dụ 1: Thêm thông tin Mã khách hàng thì tại dòng Mã trường dữ liệu/Tiện ích trên Hóa đơn Bách Khoa người dùng khai báo là NM 2</t>
@@ -465,9 +317,6 @@
 trên Hóa đơn Bách Khoa</t>
   </si>
   <si>
-    <t>HHDV 1</t>
-  </si>
-  <si>
     <t>STT</t>
   </si>
   <si>
@@ -520,9 +369,6 @@
   </si>
   <si>
     <t>Hướng dẫn nhập</t>
-  </si>
-  <si>
-    <t>Tên trường dữ liệu</t>
   </si>
   <si>
     <t>Mã Trường dữ liệu/Tiện ích
@@ -608,34 +454,154 @@
     <t>Tên nhân viên</t>
   </si>
   <si>
-    <t>HHDV 35</t>
-  </si>
-  <si>
-    <t>HHDV 36</t>
-  </si>
-  <si>
     <t>Mã nhân viên</t>
   </si>
   <si>
-    <t>DONVI</t>
-  </si>
-  <si>
-    <t>Đơn vị (*)</t>
-  </si>
-  <si>
-    <t>Thông tin đơn vị lập hóa đơn</t>
-  </si>
-  <si>
-    <t>Đơn vị</t>
-  </si>
-  <si>
-    <t>Nhập Đơn vị lập hóa đơn</t>
+    <t>Tính chất</t>
+  </si>
+  <si>
+    <t>NM1</t>
+  </si>
+  <si>
+    <t>NM3</t>
+  </si>
+  <si>
+    <t>NM4</t>
+  </si>
+  <si>
+    <t>NM5</t>
+  </si>
+  <si>
+    <t>NM6</t>
+  </si>
+  <si>
+    <t>NM7</t>
+  </si>
+  <si>
+    <t>NM9</t>
+  </si>
+  <si>
+    <t>NM10</t>
+  </si>
+  <si>
+    <t>HHDV3</t>
+  </si>
+  <si>
+    <t>HHDV4</t>
+  </si>
+  <si>
+    <t>HHDV6</t>
+  </si>
+  <si>
+    <t>HHDV8</t>
+  </si>
+  <si>
+    <t>HHDV11</t>
+  </si>
+  <si>
+    <t>HHDV12</t>
+  </si>
+  <si>
+    <t>NM2</t>
+  </si>
+  <si>
+    <t>NM8</t>
+  </si>
+  <si>
+    <t>HHDV1</t>
+  </si>
+  <si>
+    <t>HHDV2</t>
+  </si>
+  <si>
+    <t>HHDV5</t>
+  </si>
+  <si>
+    <t>HHDV7</t>
+  </si>
+  <si>
+    <t>HHDV9</t>
+  </si>
+  <si>
+    <t>HHDV10</t>
+  </si>
+  <si>
+    <t>HHDV13</t>
+  </si>
+  <si>
+    <t>HHDV14</t>
+  </si>
+  <si>
+    <t>HHDV15</t>
+  </si>
+  <si>
+    <t>HHDV16</t>
+  </si>
+  <si>
+    <t>HHDV17</t>
+  </si>
+  <si>
+    <t>HHDV18</t>
+  </si>
+  <si>
+    <t>HHDV19</t>
+  </si>
+  <si>
+    <t>HHDV20</t>
+  </si>
+  <si>
+    <t>HHDV21</t>
+  </si>
+  <si>
+    <t>HHDV22</t>
+  </si>
+  <si>
+    <t>HHDV23</t>
+  </si>
+  <si>
+    <t>HHDV24</t>
+  </si>
+  <si>
+    <t>HHDV25</t>
+  </si>
+  <si>
+    <t>HHDV26</t>
+  </si>
+  <si>
+    <t>HHDV27</t>
+  </si>
+  <si>
+    <t>HHDV28</t>
+  </si>
+  <si>
+    <t>HHDV29</t>
+  </si>
+  <si>
+    <t>HHDV30</t>
+  </si>
+  <si>
+    <t>HHDV31</t>
+  </si>
+  <si>
+    <t>HHDV32</t>
+  </si>
+  <si>
+    <t>HHDV33</t>
+  </si>
+  <si>
+    <t>HHDV34</t>
+  </si>
+  <si>
+    <t>HHDV35</t>
+  </si>
+  <si>
+    <t>HHDV36</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000\ ;[Red]\-#,##0.0000\ "/>
@@ -745,7 +711,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -779,12 +745,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -824,7 +784,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -863,7 +823,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
@@ -892,7 +851,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -904,8 +863,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Percent 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Percent 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1182,374 +1141,222 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="26.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="26.5546875" style="1"/>
-    <col min="4" max="4" width="23.44140625" style="1" customWidth="1"/>
-    <col min="5" max="8" width="26.5546875" style="1"/>
-    <col min="9" max="9" width="26.5546875" style="2"/>
-    <col min="10" max="16384" width="26.5546875" style="1"/>
+    <col min="1" max="2" width="26.5703125" style="1"/>
+    <col min="3" max="3" width="23.42578125" style="1" customWidth="1"/>
+    <col min="4" max="7" width="26.5703125" style="1"/>
+    <col min="8" max="8" width="26.5703125" style="2"/>
+    <col min="9" max="16384" width="26.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="I12" s="29" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="J12" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="K12" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="L12" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="N12" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="O12" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="P12" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q12" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="R12" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="S12" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="T12" s="29" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="D12" s="30" t="s">
+    <row r="13" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="E12" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="K12" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="L12" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="M12" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="N12" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="O12" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="P12" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q12" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="R12" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="S12" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="T12" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="U12" s="30" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="E13" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="E13" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="F13" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="G13" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="H13" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="I13" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="24" t="s">
+      <c r="J13" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="24" t="s">
+      <c r="K13" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="M13" s="24" t="s">
+      <c r="L13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="N13" s="24" t="s">
+      <c r="M13" s="23" t="s">
         <v>13</v>
       </c>
+      <c r="N13" s="23" t="s">
+        <v>14</v>
+      </c>
       <c r="O13" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="P13" s="25" t="s">
-        <v>165</v>
+        <v>114</v>
+      </c>
+      <c r="P13" s="24" t="s">
+        <v>7</v>
       </c>
       <c r="Q13" s="25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R13" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="S13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="T13" s="27" t="s">
+      <c r="S13" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="U13" s="27" t="s">
+      <c r="T13" s="26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="18"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="18"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="18"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="18"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="18"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="18"/>
-    </row>
   </sheetData>
-  <dataValidations count="22">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Không nhập thông tin tại cột này" sqref="A13:A1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập số thứ tự của hóa đơn._x000a_Lưu ý: Mỗi số thứ tự sẽ tương ứng với 1 hóa đơn_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống." sqref="B13:B1048576"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Ngày hóa đơn." sqref="E13:E1048576"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên người mua hàng" sqref="F13:F1048576"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên khách hàng" sqref="G13:G1048576"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Địa chỉ" sqref="H13:H1048576"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã số thuế_x000a_Tối đa 14 ký tự" sqref="I13:I1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Hình thức thanh toán" sqref="J13:J1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Email người nhận hóa đơn._x000a_Nếu nhiều Email thì mỗi Email cách nhau bởi dấu &quot;;&quot;" sqref="K13:K1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Số tài khoản ngân hàng" sqref="L13:L1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên ngân hàng" sqref="M13:M1048576"/>
-    <dataValidation showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã loại tiền._x000a_Nếu để trống ngầm định là VND." sqref="N13:N1048576"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tỷ giá_x000a_Tối đa 15 ký tự" sqref="O13:O1048576"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên hàng hóa, dịch vụ._x000a_Trường dữ liệu bắt buộc._x000a_Không để trống" sqref="P13:P1048576"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn vị tính." sqref="Q13:Q1048576"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền quy đổi_x000a_Tối đa 15 ký tự" sqref="U13:U1048576"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền_x000a_Tối đa 15 ký tự" sqref="T13:T1048576"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn giá_x000a_Tối đa 15 ký tự" sqref="S13:S1048576"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Số lượng_x000a_Tối đa 15 ký tự" sqref="R13:R1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã trường dữ liệu/Tiện ích tương ứng trên Hóa đơn Bách Khoa" sqref="C12:U12"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã nhân viên bán hàng._x000a_Lưu ý:_x000a_Để trống nếu không thiết lập Tùy chọn/Quản lý nhân viên bán hàng trên hóa đơn._x000a_Nhập theo danh mục đã tạo tại Danh mục/Nhân viên" sqref="D13:D1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã đơn vị lập hóa đơn._x000a_Lưu ý:_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống._x000a_Nhập theo danh mục đã tạo tại Danh mục/Cơ cấu tổ chức" sqref="C13 C14:C1048576"/>
+  <dataValidations count="21">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập số thứ tự của hóa đơn._x000a_Lưu ý: Mỗi số thứ tự sẽ tương ứng với 1 hóa đơn_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống." sqref="B13:B1048576" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Ngày hóa đơn." sqref="D13:D1048576" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên người mua hàng" sqref="E13:E1048576" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên khách hàng" sqref="F13:F1048576" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Địa chỉ" sqref="G13:G1048576" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã số thuế_x000a_Tối đa 14 ký tự" sqref="H13:H1048576" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Hình thức thanh toán" sqref="I13:I1048576" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Email người nhận hóa đơn._x000a_Nếu nhiều Email thì mỗi Email cách nhau bởi dấu &quot;;&quot;" sqref="J13:J1048576" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Số tài khoản ngân hàng" sqref="K13:K1048576" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên ngân hàng" sqref="L13:L1048576" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã loại tiền._x000a_Nếu để trống ngầm định là VND." sqref="M13:M1048576" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tỷ giá_x000a_Tối đa 15 ký tự" sqref="N13:N1048576" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên hàng hóa, dịch vụ._x000a_Trường dữ liệu bắt buộc._x000a_Không để trống" sqref="O13:O1048576" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn vị tính." sqref="P13:P1048576" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền quy đổi_x000a_Tối đa 15 ký tự" sqref="T13:T1048576" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền_x000a_Tối đa 15 ký tự" sqref="S13:S1048576" xr:uid="{00000000-0002-0000-0000-000010000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn giá_x000a_Tối đa 15 ký tự" sqref="R13:R1048576" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Số lượng_x000a_Tối đa 15 ký tự" sqref="Q13:Q1048576" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã nhân viên bán hàng._x000a_Lưu ý:_x000a_Để trống nếu không thiết lập Tùy chọn/Quản lý nhân viên bán hàng trên hóa đơn._x000a_Nhập theo danh mục đã tạo tại Danh mục/Nhân viên" sqref="C13:C1048576" xr:uid="{00000000-0002-0000-0000-000014000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tính chất._x000a_Trường dữ liệu bắt buộc._x000a_Không để trống._x000a_Nhập 1: Hàng hóa, dịch vụ._x000a_Nhập 2: Khuyến mại._x000a_Nhập 3: Chiết khấu._x000a_Nhập 4: Ghi chú/diễn giải._x000a_" sqref="A12:A1048576" xr:uid="{DDBE8857-7DAA-4B68-AA52-2071A6BF58D3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã trường dữ liệu/Tiện ích tương ứng trên Hóa đơn Bách Khoa" sqref="C12:T12" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1557,96 +1364,96 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" customWidth="1"/>
-    <col min="3" max="3" width="44.21875" customWidth="1"/>
-    <col min="4" max="4" width="71.21875" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="4" max="4" width="71.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
-        <v>163</v>
+    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>162</v>
+      <c r="A2" s="19" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>168</v>
+      <c r="A3" s="19" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-    </row>
-    <row r="6" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+    </row>
+    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>161</v>
+        <v>110</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>140</v>
+        <v>91</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>179</v>
+        <v>55</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>177</v>
+        <v>81</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>180</v>
+        <v>1</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>181</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>98</v>
+      <c r="A9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1654,13 +1461,13 @@
         <v>37</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1668,13 +1475,13 @@
         <v>37</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>43</v>
+        <v>126</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>131</v>
+        <v>12</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>132</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1682,83 +1489,83 @@
         <v>37</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>45</v>
+        <v>128</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>47</v>
+        <v>130</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>48</v>
+        <v>140</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>49</v>
+        <v>131</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>108</v>
+        <v>40</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1766,97 +1573,97 @@
         <v>37</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>50</v>
+        <v>132</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>121</v>
+        <v>80</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="C22" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>141</v>
-      </c>
       <c r="C24" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>117</v>
+        <v>22</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1864,41 +1671,41 @@
         <v>38</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>51</v>
+        <v>143</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>52</v>
+        <v>135</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>53</v>
+        <v>144</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1906,69 +1713,69 @@
         <v>38</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>54</v>
+        <v>136</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>55</v>
+        <v>145</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>56</v>
+        <v>146</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>57</v>
+        <v>137</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1976,125 +1783,125 @@
         <v>38</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>59</v>
+        <v>147</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>60</v>
+        <v>148</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>61</v>
+        <v>149</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>116</v>
+      <c r="A36" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>171</v>
+      <c r="A39" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>171</v>
+      <c r="A40" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C41" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>171</v>
+      <c r="A41" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2102,13 +1909,13 @@
         <v>38</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>68</v>
+        <v>156</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2116,13 +1923,13 @@
         <v>38</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>69</v>
+        <v>157</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>144</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2130,13 +1937,13 @@
         <v>38</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2144,13 +1951,13 @@
         <v>38</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>71</v>
+        <v>159</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>146</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2158,13 +1965,13 @@
         <v>38</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>147</v>
+        <v>122</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2172,13 +1979,13 @@
         <v>38</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>73</v>
+        <v>161</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2186,13 +1993,13 @@
         <v>38</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>74</v>
+        <v>162</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>176</v>
+        <v>46</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2200,13 +2007,13 @@
         <v>38</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>75</v>
+        <v>163</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>117</v>
+        <v>47</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2214,13 +2021,13 @@
         <v>38</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>76</v>
+        <v>164</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2228,13 +2035,13 @@
         <v>38</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2242,13 +2049,13 @@
         <v>38</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>78</v>
+        <v>166</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>151</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2256,13 +2063,13 @@
         <v>38</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>79</v>
+        <v>167</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>152</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2270,13 +2077,13 @@
         <v>38</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>80</v>
+        <v>168</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>153</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2284,13 +2091,13 @@
         <v>38</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2298,62 +2105,20 @@
         <v>38</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>82</v>
+        <v>170</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B58" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B59" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Feature #539: Cập nhật form lập hóa đơn Chiết khấu + Giảm thuế + Nhập khẩu Excel
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
+++ b/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\Template\ImportHoaDon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB66F4E-BCC9-4621-ADD0-3B70A9BFDCA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B1D710-3EC3-4525-9FC4-39C2A5CA6125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,25 @@
     <sheet name="Hóa đơn bán hàng" sheetId="1" r:id="rId1"/>
     <sheet name="Nguyên tắc ghép dữ liệu" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="184">
   <si>
     <t>Số thứ tự hóa đơn (*)</t>
   </si>
@@ -599,6 +607,45 @@
   </si>
   <si>
     <t>Tỷ lệ chiết khấu (%)</t>
+  </si>
+  <si>
+    <t>HHDV37</t>
+  </si>
+  <si>
+    <t>HHDV38</t>
+  </si>
+  <si>
+    <t>HHDV39</t>
+  </si>
+  <si>
+    <t>Trường Tỷ lệ % trên doanh thu</t>
+  </si>
+  <si>
+    <t>Trường Tiền giảm 20% mức tỷ lệ</t>
+  </si>
+  <si>
+    <t>Trường Tiền giảm 20% mức tỷ lệ quy đổi</t>
+  </si>
+  <si>
+    <t>Nhập Tiền giảm 20% mức tỷ lệ
+Tối đa 15 ký tự</t>
+  </si>
+  <si>
+    <t>Nhập Tiền giảm 20% mức tỷ lệ quy đổi
+Tối đa 15 ký tự</t>
+  </si>
+  <si>
+    <t>Nhập Tỷ lệ % trên doanh thu.
+Lớn hơn 0 và lập riêng hóa đơn cho từng tỷ lệ % trên doanh thu.</t>
+  </si>
+  <si>
+    <t>Tỷ lệ % trên doanh thu</t>
+  </si>
+  <si>
+    <t>Tiền giảm 20% mức tỷ lệ</t>
+  </si>
+  <si>
+    <t>Tiền giảm 20% mức tỷ lệ quy đổi</t>
   </si>
 </sst>
 </file>
@@ -788,7 +835,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -866,6 +913,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1147,11 +1197,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,10 +1214,11 @@
     <col min="9" max="9" width="26.5703125" style="1"/>
     <col min="10" max="12" width="26.5703125" style="30"/>
     <col min="13" max="20" width="26.5703125" style="1"/>
-    <col min="24" max="16384" width="26.5703125" style="1"/>
+    <col min="26" max="26" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="26.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -1181,8 +1232,11 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>86</v>
       </c>
@@ -1196,8 +1250,11 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
@@ -1211,8 +1268,11 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>121</v>
       </c>
@@ -1226,8 +1286,11 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -1241,8 +1304,11 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>83</v>
       </c>
@@ -1256,8 +1322,11 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>113</v>
       </c>
@@ -1271,8 +1340,11 @@
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>89</v>
       </c>
@@ -1286,8 +1358,11 @@
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>87</v>
       </c>
@@ -1301,8 +1376,11 @@
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>88</v>
       </c>
@@ -1316,8 +1394,11 @@
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1329,8 +1410,11 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
-    </row>
-    <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+    </row>
+    <row r="12" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
         <v>90</v>
       </c>
@@ -1400,8 +1484,17 @@
       <c r="W12" s="29" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X12" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y12" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z12" s="29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>124</v>
       </c>
@@ -1471,33 +1564,45 @@
       <c r="W13" s="26" t="s">
         <v>28</v>
       </c>
+      <c r="X13" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y13" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z13" s="26" t="s">
+        <v>183</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="24">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập số thứ tự của hóa đơn._x000a_Lưu ý: Mỗi số thứ tự sẽ tương ứng với 1 hóa đơn_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống." sqref="B13:B1048576" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Ngày hóa đơn." sqref="D13:D1048576" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên người mua hàng" sqref="E13:E1048576" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên khách hàng" sqref="F13:F1048576" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Địa chỉ" sqref="G13:G1048576" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã số thuế_x000a_Tối đa 14 ký tự" sqref="H13:H1048576" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Hình thức thanh toán_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống._x000a_Nhập 1: Tiền mặt_x000a_Nhập 2: Chuyển khoản_x000a_Nhập 3: Tiền mặt/Chuyển khoản_x000a_Nhập 4: Đối trừ công nợ_x000a_Nhập 5: Không thu tiền_x000a_Nhập 6: Khác" sqref="I13:I1048576" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Email người nhận hóa đơn._x000a_Nếu nhiều Email thì mỗi Email cách nhau bởi dấu &quot;;&quot;" sqref="J13:J1048576" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Số tài khoản ngân hàng" sqref="K13:K1048576" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên ngân hàng" sqref="L13:L1048576" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã loại tiền._x000a_Nếu để trống ngầm định là VND." sqref="M13:M1048576" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tỷ giá_x000a_Tối đa 15 ký tự" sqref="N13:N1048576" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên hàng hóa, dịch vụ._x000a_Trường dữ liệu bắt buộc._x000a_Không để trống" sqref="O13:O1048576" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn vị tính." sqref="P13:P1048576" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền quy đổi_x000a_Tối đa 15 ký tự" sqref="T13:T1048576" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền_x000a_Tối đa 15 ký tự" sqref="S13:S1048576" xr:uid="{00000000-0002-0000-0000-000010000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn giá_x000a_Tối đa 15 ký tự" sqref="R13:R1048576" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Số lượng_x000a_Tối đa 15 ký tự" sqref="Q13:Q1048576" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã nhân viên bán hàng._x000a_Lưu ý:_x000a_Để trống nếu không thiết lập Tùy chọn/Quản lý nhân viên bán hàng trên hóa đơn._x000a_Nhập theo danh mục đã tạo tại Danh mục/Nhân viên" sqref="C13:C1048576" xr:uid="{00000000-0002-0000-0000-000014000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tính chất._x000a_Trường dữ liệu bắt buộc._x000a_Không để trống._x000a_Nhập 1: Hàng hóa, dịch vụ._x000a_Nhập 2: Khuyến mại._x000a_Nhập 3: Chiết khấu._x000a_Nhập 4: Ghi chú/diễn giải._x000a_" sqref="A12:A1048576" xr:uid="{DDBE8857-7DAA-4B68-AA52-2071A6BF58D3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã trường dữ liệu/Tiện ích tương ứng trên Hóa đơn Bách Khoa" sqref="C12:W12" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền chiết khấu quy đổi._x000a_Tối đa 15 ký tự." sqref="W13:W1048573" xr:uid="{68E654C8-EE10-43D3-9C7F-4B511C11B598}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền chiết khấu._x000a_Tối đa 15 ký tự" sqref="V13:V1048573" xr:uid="{E3479629-C6FC-4FF1-B0BA-3A3E006DF32F}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tỷ lệ chiết khấu (%)." sqref="U13 U15:U1048573 W14" xr:uid="{29A8265A-FD95-41B8-9FC4-4E6408D51876}"/>
+  <dataValidations count="27">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập số thứ tự của hóa đơn._x000a_Lưu ý: Mỗi số thứ tự sẽ tương ứng với 1 hóa đơn_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống." sqref="B13:B1048576" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Ngày hóa đơn." sqref="D13:D1048576" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên người mua hàng" sqref="E13:E1048576" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên khách hàng" sqref="F13:F1048576" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Địa chỉ" sqref="G13:G1048576" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã số thuế_x000a_Tối đa 14 ký tự" sqref="H13:H1048576" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Hình thức thanh toán_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống._x000a_Nhập 1: Tiền mặt_x000a_Nhập 2: Chuyển khoản_x000a_Nhập 3: Tiền mặt/Chuyển khoản_x000a_Nhập 4: Đối trừ công nợ_x000a_Nhập 5: Không thu tiền_x000a_Nhập 6: Khác" sqref="I13:I1048576" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Email người nhận hóa đơn._x000a_Nếu nhiều Email thì mỗi Email cách nhau bởi dấu &quot;;&quot;" sqref="J13:J1048576" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Số tài khoản ngân hàng" sqref="K13:K1048576" xr:uid="{00000000-0002-0000-0100-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên ngân hàng" sqref="L13:L1048576" xr:uid="{00000000-0002-0000-0100-000009000000}"/>
+    <dataValidation showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã loại tiền._x000a_Nếu để trống ngầm định là VND." sqref="M13:M1048576" xr:uid="{00000000-0002-0000-0100-00000A000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tỷ giá_x000a_Tối đa 15 ký tự" sqref="N13:N1048576" xr:uid="{00000000-0002-0000-0100-00000B000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên hàng hóa, dịch vụ._x000a_Trường dữ liệu bắt buộc._x000a_Không để trống" sqref="O13:O1048576" xr:uid="{00000000-0002-0000-0100-00000C000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn vị tính." sqref="P13:P1048576" xr:uid="{00000000-0002-0000-0100-00000D000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền quy đổi_x000a_Tối đa 15 ký tự" sqref="T13:T1048576" xr:uid="{00000000-0002-0000-0100-00000E000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền_x000a_Tối đa 15 ký tự" sqref="S13:S1048576" xr:uid="{00000000-0002-0000-0100-00000F000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn giá_x000a_Tối đa 15 ký tự" sqref="R13:R1048576" xr:uid="{00000000-0002-0000-0100-000010000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Số lượng_x000a_Tối đa 15 ký tự" sqref="Q13:Q1048576" xr:uid="{00000000-0002-0000-0100-000011000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã nhân viên bán hàng._x000a_Lưu ý:_x000a_Để trống nếu không thiết lập Tùy chọn/Quản lý nhân viên bán hàng trên hóa đơn._x000a_Nhập theo danh mục đã tạo tại Danh mục/Nhân viên" sqref="C13:C1048576" xr:uid="{00000000-0002-0000-0100-000012000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tính chất._x000a_Trường dữ liệu bắt buộc._x000a_Không để trống._x000a_Nhập 1: Hàng hóa, dịch vụ._x000a_Nhập 2: Khuyến mại._x000a_Nhập 3: Chiết khấu._x000a_Nhập 4: Ghi chú/diễn giải._x000a_" sqref="A12:A1048576" xr:uid="{00000000-0002-0000-0100-000013000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã trường dữ liệu/Tiện ích tương ứng trên Hóa đơn Bách Khoa" sqref="C12:Z12" xr:uid="{00000000-0002-0000-0100-000014000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền chiết khấu quy đổi._x000a_Tối đa 15 ký tự." sqref="W13" xr:uid="{00000000-0002-0000-0100-000015000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền chiết khấu._x000a_Tối đa 15 ký tự" sqref="V13" xr:uid="{00000000-0002-0000-0100-000016000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tỷ lệ chiết khấu (%)." sqref="U13" xr:uid="{00000000-0002-0000-0100-000017000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tỷ lệ % trên doanh thu._x000a_Lớn hơn 0 và lập riêng hóa đơn cho từng tỷ lệ % trên doanh thu." sqref="X13:X1048576" xr:uid="{EFE383E8-B6A4-4218-A809-9805BED566E1}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền giảm 20% mức tỷ lệ._x000a_Tối đa 15 ký tự." sqref="Y13:Y1048576" xr:uid="{5DB40F09-29F8-44BA-B05A-8A81544C8B18}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền giảm 20% mức tỷ lệ quy đổi._x000a_Tối đa 15 ký tự." sqref="Z13:Z1048576" xr:uid="{DFEA5F7B-80E5-48BB-95ED-818CA4786A6C}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1505,14 +1610,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView showGridLines="0" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2255,11 +2360,53 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Feature #1812: Mo ta trinh bay thue suat 8 - LK 2022-06-21
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
+++ b/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\Telegram Desktop\Giam thue 8 - Cap nhat theo ND 41-2022-ND-CP ngay 20.06.2022\Giam thue 8 - Cap nhat theo ND 41-2022-ND-CP ngay 20.06.2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B1D710-3EC3-4525-9FC4-39C2A5CA6125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AC52CC-7186-4ED1-9DA1-011471EA2BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,25 +16,17 @@
     <sheet name="Hóa đơn bán hàng" sheetId="1" r:id="rId1"/>
     <sheet name="Nguyên tắc ghép dữ liệu" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="183">
   <si>
     <t>Số thứ tự hóa đơn (*)</t>
   </si>
@@ -100,9 +92,6 @@
   </si>
   <si>
     <t>Tên hàng</t>
-  </si>
-  <si>
-    <t>Hàng khuyến mại</t>
   </si>
   <si>
     <t>Mã quy cách</t>
@@ -240,10 +229,6 @@
 Nếu nhiều số điện thoại thì mỗi số điện thoại cách nhau bởi dấu ";"</t>
   </si>
   <si>
-    <t>Nhập 0 hoặc để trống nếu không là Hàng khuyến mại
-Nhâp 1 nếu là Hàng khuyến mại</t>
-  </si>
-  <si>
     <t>Nhập Đơn vị tính</t>
   </si>
   <si>
@@ -306,12 +291,6 @@
   </si>
   <si>
     <t>- Khai báo dữ liệu hóa đơn cần lập trên Hóa đơn Bách Khoa tại các cột tương ứng trên file này</t>
-  </si>
-  <si>
-    <t>Ví dụ 1: Thêm thông tin Mã khách hàng thì tại dòng Mã trường dữ liệu/Tiện ích trên Hóa đơn Bách Khoa người dùng khai báo là NM 2</t>
-  </si>
-  <si>
-    <t>Ví dụ 2: Đánh dấu dòng khai báo là dòng chiết khấu thì thêm cột thông tin Là dòng chiết khấu và tại dòng Mã trường dữ liệu/Tiện ích trên Hóa đơn Bách Khoa người dùng khai báo là DONGCHIETKHAU</t>
   </si>
   <si>
     <t xml:space="preserve">+ Hệ thống căn cứ vào dòng mã này để ghép dữ liệu hóa đơn đã khai báo đúng Trường dữ liệu/Tiện ích tương ứng trên Hóa đơn Bách Khoa </t>
@@ -468,154 +447,7 @@
     <t>Tính chất</t>
   </si>
   <si>
-    <t>NM1</t>
-  </si>
-  <si>
-    <t>NM3</t>
-  </si>
-  <si>
-    <t>NM4</t>
-  </si>
-  <si>
-    <t>NM5</t>
-  </si>
-  <si>
-    <t>NM6</t>
-  </si>
-  <si>
-    <t>NM7</t>
-  </si>
-  <si>
-    <t>NM9</t>
-  </si>
-  <si>
-    <t>NM10</t>
-  </si>
-  <si>
-    <t>HHDV3</t>
-  </si>
-  <si>
-    <t>HHDV4</t>
-  </si>
-  <si>
-    <t>HHDV6</t>
-  </si>
-  <si>
-    <t>HHDV8</t>
-  </si>
-  <si>
-    <t>HHDV11</t>
-  </si>
-  <si>
-    <t>HHDV12</t>
-  </si>
-  <si>
-    <t>NM2</t>
-  </si>
-  <si>
-    <t>NM8</t>
-  </si>
-  <si>
-    <t>HHDV1</t>
-  </si>
-  <si>
-    <t>HHDV2</t>
-  </si>
-  <si>
-    <t>HHDV5</t>
-  </si>
-  <si>
-    <t>HHDV7</t>
-  </si>
-  <si>
-    <t>HHDV9</t>
-  </si>
-  <si>
-    <t>HHDV10</t>
-  </si>
-  <si>
-    <t>HHDV13</t>
-  </si>
-  <si>
-    <t>HHDV14</t>
-  </si>
-  <si>
-    <t>HHDV15</t>
-  </si>
-  <si>
-    <t>HHDV16</t>
-  </si>
-  <si>
-    <t>HHDV17</t>
-  </si>
-  <si>
-    <t>HHDV18</t>
-  </si>
-  <si>
-    <t>HHDV19</t>
-  </si>
-  <si>
-    <t>HHDV20</t>
-  </si>
-  <si>
-    <t>HHDV21</t>
-  </si>
-  <si>
-    <t>HHDV22</t>
-  </si>
-  <si>
-    <t>HHDV23</t>
-  </si>
-  <si>
-    <t>HHDV24</t>
-  </si>
-  <si>
-    <t>HHDV25</t>
-  </si>
-  <si>
-    <t>HHDV26</t>
-  </si>
-  <si>
-    <t>HHDV27</t>
-  </si>
-  <si>
-    <t>HHDV28</t>
-  </si>
-  <si>
-    <t>HHDV29</t>
-  </si>
-  <si>
-    <t>HHDV30</t>
-  </si>
-  <si>
-    <t>HHDV31</t>
-  </si>
-  <si>
-    <t>HHDV32</t>
-  </si>
-  <si>
-    <t>HHDV33</t>
-  </si>
-  <si>
-    <t>HHDV34</t>
-  </si>
-  <si>
-    <t>HHDV35</t>
-  </si>
-  <si>
-    <t>HHDV36</t>
-  </si>
-  <si>
     <t>Tỷ lệ chiết khấu (%)</t>
-  </si>
-  <si>
-    <t>HHDV37</t>
-  </si>
-  <si>
-    <t>HHDV38</t>
-  </si>
-  <si>
-    <t>HHDV39</t>
   </si>
   <si>
     <t>Trường Tỷ lệ % trên doanh thu</t>
@@ -635,17 +467,201 @@
 Tối đa 15 ký tự</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Nhập Tính chất:
+- Nhập 1 hoặc để trống: Hàng hóa, dịch vụ
+- Nhập 2: Khuyến mại
+- Nhập 3: Chiết khấu thương mại
+- Nhập 4: Ghi chú/Diễn giải
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>SỬ DỤNG CỘT A KHI NHẬP KHẨU DỮ LIỆU TỪ EXCEL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Tính chất (*)</t>
+  </si>
+  <si>
+    <t>Ví dụ: Thêm thông tin Mã khách hàng thì tại dòng Mã trường dữ liệu/Tiện ích trên Hóa đơn Bách Khoa người dùng khai báo là NM 2</t>
+  </si>
+  <si>
+    <t>Lưu ý: Không áp dụng nguyên tắc ghép dữ liệu này cho thông tin Tính chất (mã trường dữ liệu HHDV4). Tính chất hàng hóa luôn lấy thông tin tại cột A</t>
+  </si>
+  <si>
+    <t>NM 1</t>
+  </si>
+  <si>
+    <t>NM 3</t>
+  </si>
+  <si>
+    <t>NM 4</t>
+  </si>
+  <si>
+    <t>NM 5</t>
+  </si>
+  <si>
+    <t>NM 6</t>
+  </si>
+  <si>
+    <t>NM 7</t>
+  </si>
+  <si>
+    <t>NM 9</t>
+  </si>
+  <si>
+    <t>NM 10</t>
+  </si>
+  <si>
+    <t>HHDV 3</t>
+  </si>
+  <si>
+    <t>HHDV 6</t>
+  </si>
+  <si>
+    <t>HHDV 7</t>
+  </si>
+  <si>
+    <t>HHDV 9</t>
+  </si>
+  <si>
+    <t>HHDV 11</t>
+  </si>
+  <si>
+    <t>HHDV 12</t>
+  </si>
+  <si>
+    <t>HHDV 13</t>
+  </si>
+  <si>
+    <t>HHDV 14</t>
+  </si>
+  <si>
+    <t>HHDV 15</t>
+  </si>
+  <si>
+    <t>NM 2</t>
+  </si>
+  <si>
+    <t>NM 8</t>
+  </si>
+  <si>
+    <t>HHDV 1</t>
+  </si>
+  <si>
+    <t>HHDV 2</t>
+  </si>
+  <si>
+    <t>HHDV 4</t>
+  </si>
+  <si>
+    <t>HHDV 5</t>
+  </si>
+  <si>
+    <t>HHDV 8</t>
+  </si>
+  <si>
+    <t>HHDV 10</t>
+  </si>
+  <si>
+    <t>HHDV 16</t>
+  </si>
+  <si>
+    <t>HHDV 17</t>
+  </si>
+  <si>
+    <t>HHDV 18</t>
+  </si>
+  <si>
+    <t>HHDV 19</t>
+  </si>
+  <si>
+    <t>HHDV 20</t>
+  </si>
+  <si>
+    <t>HHDV 21</t>
+  </si>
+  <si>
+    <t>HHDV 22</t>
+  </si>
+  <si>
+    <t>HHDV 23</t>
+  </si>
+  <si>
+    <t>HHDV 24</t>
+  </si>
+  <si>
+    <t>HHDV 25</t>
+  </si>
+  <si>
+    <t>HHDV 26</t>
+  </si>
+  <si>
+    <t>HHDV 27</t>
+  </si>
+  <si>
+    <t>HHDV 28</t>
+  </si>
+  <si>
+    <t>HHDV 29</t>
+  </si>
+  <si>
+    <t>HHDV 30</t>
+  </si>
+  <si>
+    <t>HHDV 31</t>
+  </si>
+  <si>
+    <t>HHDV 32</t>
+  </si>
+  <si>
+    <t>HHDV 33</t>
+  </si>
+  <si>
+    <t>HHDV 34</t>
+  </si>
+  <si>
+    <t>HHDV 35</t>
+  </si>
+  <si>
+    <t>HHDV 36</t>
+  </si>
+  <si>
+    <t>HHDV 37</t>
+  </si>
+  <si>
+    <t>HHDV 38</t>
+  </si>
+  <si>
+    <t>HHDV 39</t>
+  </si>
+  <si>
+    <t>Trường Mặt hàng giảm</t>
+  </si>
+  <si>
+    <t>Nhập là Mặt hàng giảm/Mặt hàng không giảm
+- Nhập 1: Mặt hàng giảm
+- Nhập 0 hoặc Để trống: Mặt hàng không giảm</t>
+  </si>
+  <si>
     <t>Nhập Tỷ lệ % trên doanh thu.
-Lớn hơn 0 và lập riêng hóa đơn cho từng tỷ lệ % trên doanh thu.</t>
-  </si>
-  <si>
-    <t>Tỷ lệ % trên doanh thu</t>
-  </si>
-  <si>
-    <t>Tiền giảm 20% mức tỷ lệ</t>
-  </si>
-  <si>
-    <t>Tiền giảm 20% mức tỷ lệ quy đổi</t>
+Lớn hơn 0</t>
   </si>
 </sst>
 </file>
@@ -656,7 +672,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000\ ;[Red]\-#,##0.0000\ "/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -761,6 +777,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -835,7 +858,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -913,6 +936,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1198,10 +1227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,11 +1243,10 @@
     <col min="9" max="9" width="26.5703125" style="1"/>
     <col min="10" max="12" width="26.5703125" style="30"/>
     <col min="13" max="20" width="26.5703125" style="1"/>
-    <col min="26" max="26" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="26.5703125" style="1"/>
+    <col min="24" max="16384" width="26.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -1232,13 +1260,10 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1250,11 +1275,8 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
@@ -1268,13 +1290,10 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1286,11 +1305,8 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -1304,13 +1320,10 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1322,13 +1335,10 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1340,13 +1350,10 @@
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1358,13 +1365,10 @@
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1376,13 +1380,10 @@
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>88</v>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>130</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1394,11 +1395,8 @@
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1410,99 +1408,87 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-    </row>
-    <row r="12" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="H12" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="J12" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="K12" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="L12" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N12" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="O12" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="P12" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q12" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="R12" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="S12" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="T12" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="U12" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="V12" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="W12" s="29" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
         <v>128</v>
-      </c>
-      <c r="I12" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="J12" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="K12" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="L12" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="M12" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N12" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="O12" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="P12" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q12" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="R12" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="S12" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="T12" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="U12" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="V12" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="W12" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="X12" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="Y12" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="Z12" s="29" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>124</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>1</v>
@@ -1526,10 +1512,10 @@
         <v>5</v>
       </c>
       <c r="K13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="23" t="s">
         <v>40</v>
-      </c>
-      <c r="L13" s="23" t="s">
-        <v>41</v>
       </c>
       <c r="M13" s="23" t="s">
         <v>13</v>
@@ -1538,7 +1524,7 @@
         <v>14</v>
       </c>
       <c r="O13" s="24" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="P13" s="24" t="s">
         <v>7</v>
@@ -1556,26 +1542,17 @@
         <v>15</v>
       </c>
       <c r="U13" s="26" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="V13" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="W13" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="W13" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="X13" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="Y13" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z13" s="26" t="s">
-        <v>183</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="27">
+  <dataValidations count="24">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập số thứ tự của hóa đơn._x000a_Lưu ý: Mỗi số thứ tự sẽ tương ứng với 1 hóa đơn_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống." sqref="B13:B1048576" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Ngày hóa đơn." sqref="D13:D1048576" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên người mua hàng" sqref="E13:E1048576" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
@@ -1595,14 +1572,11 @@
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn giá_x000a_Tối đa 15 ký tự" sqref="R13:R1048576" xr:uid="{00000000-0002-0000-0100-000010000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Số lượng_x000a_Tối đa 15 ký tự" sqref="Q13:Q1048576" xr:uid="{00000000-0002-0000-0100-000011000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã nhân viên bán hàng._x000a_Lưu ý:_x000a_Để trống nếu không thiết lập Tùy chọn/Quản lý nhân viên bán hàng trên hóa đơn._x000a_Nhập theo danh mục đã tạo tại Danh mục/Nhân viên" sqref="C13:C1048576" xr:uid="{00000000-0002-0000-0100-000012000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tính chất._x000a_Trường dữ liệu bắt buộc._x000a_Không để trống._x000a_Nhập 1: Hàng hóa, dịch vụ._x000a_Nhập 2: Khuyến mại._x000a_Nhập 3: Chiết khấu._x000a_Nhập 4: Ghi chú/diễn giải._x000a_" sqref="A12:A1048576" xr:uid="{00000000-0002-0000-0100-000013000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã trường dữ liệu/Tiện ích tương ứng trên Hóa đơn Bách Khoa" sqref="C12:Z12" xr:uid="{00000000-0002-0000-0100-000014000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền chiết khấu quy đổi._x000a_Tối đa 15 ký tự." sqref="W13" xr:uid="{00000000-0002-0000-0100-000015000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền chiết khấu._x000a_Tối đa 15 ký tự" sqref="V13" xr:uid="{00000000-0002-0000-0100-000016000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tỷ lệ chiết khấu (%)." sqref="U13" xr:uid="{00000000-0002-0000-0100-000017000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tỷ lệ % trên doanh thu._x000a_Lớn hơn 0 và lập riêng hóa đơn cho từng tỷ lệ % trên doanh thu." sqref="X13:X1048576" xr:uid="{EFE383E8-B6A4-4218-A809-9805BED566E1}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền giảm 20% mức tỷ lệ._x000a_Tối đa 15 ký tự." sqref="Y13:Y1048576" xr:uid="{5DB40F09-29F8-44BA-B05A-8A81544C8B18}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền giảm 20% mức tỷ lệ quy đổi._x000a_Tối đa 15 ký tự." sqref="Z13:Z1048576" xr:uid="{DFEA5F7B-80E5-48BB-95ED-818CA4786A6C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tính chất:_x000a_Nhập 1 hoặc Để trống: Hàng hóa, dịch vụ_x000a_Nhập 2: Khuyến mại_x000a_Nhập 3: Chiết khấu thương mại_x000a_Nhập 4: Ghi chú/diễn giải._x000a_" sqref="A12:A1048576" xr:uid="{00000000-0002-0000-0100-000013000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã trường dữ liệu/Tiện ích tương ứng trên Hóa đơn Bách Khoa" sqref="C12:W12" xr:uid="{00000000-0002-0000-0100-000014000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền chiết khấu quy đổi._x000a_Tối đa 15 ký tự." sqref="W13:W1048573" xr:uid="{00000000-0002-0000-0100-000015000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tiền chiết khấu._x000a_Tối đa 15 ký tự" sqref="V13:V1048573" xr:uid="{00000000-0002-0000-0100-000016000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tỷ lệ chiết khấu (%)." sqref="U13 U15:U1048573 W14" xr:uid="{00000000-0002-0000-0100-000017000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1614,10 +1588,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView showGridLines="0" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,17 +1604,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1648,765 +1622,779 @@
     </row>
     <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>67</v>
+        <v>120</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>16</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="D58" s="32" t="s">
-        <v>178</v>
+        <v>122</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="D59" s="32" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
+        <v>123</v>
+      </c>
+      <c r="D59" s="34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D60" s="34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update file import hoa don ban hang
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
+++ b/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\Telegram Desktop\Giam thue 8 - Cap nhat theo ND 41-2022-ND-CP ngay 20.06.2022\Giam thue 8 - Cap nhat theo ND 41-2022-ND-CP ngay 20.06.2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\BKSoft\bill-back-end\API\wwwroot\docs\Template\ImportHoaDon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AC52CC-7186-4ED1-9DA1-011471EA2BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A52AEA2-F358-4B7C-98C8-25DFBFC898F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hóa đơn bán hàng" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="184">
   <si>
     <t>Số thứ tự hóa đơn (*)</t>
   </si>
@@ -662,6 +662,9 @@
   <si>
     <t>Nhập Tỷ lệ % trên doanh thu.
 Lớn hơn 0</t>
+  </si>
+  <si>
+    <t>HHDV 40</t>
   </si>
 </sst>
 </file>
@@ -1233,17 +1236,17 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="26.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="26.5703125" style="1"/>
-    <col min="3" max="3" width="23.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" style="1"/>
-    <col min="5" max="7" width="26.5703125" style="30"/>
-    <col min="8" max="8" width="26.5703125" style="31"/>
-    <col min="9" max="9" width="26.5703125" style="1"/>
-    <col min="10" max="12" width="26.5703125" style="30"/>
-    <col min="13" max="20" width="26.5703125" style="1"/>
-    <col min="24" max="16384" width="26.5703125" style="1"/>
+    <col min="1" max="2" width="26.5546875" style="1"/>
+    <col min="3" max="3" width="23.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" style="1"/>
+    <col min="5" max="7" width="26.5546875" style="30"/>
+    <col min="8" max="8" width="26.5546875" style="31"/>
+    <col min="9" max="9" width="26.5546875" style="1"/>
+    <col min="10" max="12" width="26.5546875" style="30"/>
+    <col min="13" max="20" width="26.5546875" style="1"/>
+    <col min="24" max="16384" width="26.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -1409,7 +1412,7 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
         <v>86</v>
       </c>
@@ -1590,19 +1593,19 @@
   </sheetPr>
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" customWidth="1"/>
-    <col min="4" max="4" width="71.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="4" max="4" width="71.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>108</v>
       </c>
@@ -1620,7 +1623,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
     </row>
-    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>35</v>
       </c>
@@ -1718,7 +1721,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>36</v>
       </c>
@@ -1746,7 +1749,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>36</v>
       </c>
@@ -1760,7 +1763,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
@@ -1802,7 +1805,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>41</v>
       </c>
@@ -1816,7 +1819,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>41</v>
       </c>
@@ -1858,7 +1861,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>37</v>
       </c>
@@ -1872,7 +1875,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>37</v>
       </c>
@@ -1914,7 +1917,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>37</v>
       </c>
@@ -1942,7 +1945,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>37</v>
       </c>
@@ -1970,7 +1973,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>37</v>
       </c>
@@ -1984,7 +1987,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>37</v>
       </c>
@@ -2012,7 +2015,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>37</v>
       </c>
@@ -2026,7 +2029,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>37</v>
       </c>
@@ -2334,7 +2337,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>37</v>
       </c>
@@ -2348,7 +2351,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>37</v>
       </c>
@@ -2362,7 +2365,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>37</v>
       </c>
@@ -2376,12 +2379,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>124</v>

</xml_diff>

<commit_message>
Bug #1842: ND41-Mo ta trinh bay thue suat 8 - Nghiem thu 2022-06-25
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
+++ b/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
@@ -5,21 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\Telegram Desktop\Giam thue 8 - Cap nhat theo ND 41-2022-ND-CP ngay 20.06.2022\Giam thue 8 - Cap nhat theo ND 41-2022-ND-CP ngay 20.06.2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\Template\ImportHoaDon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AC52CC-7186-4ED1-9DA1-011471EA2BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66D6DC4-E25A-4C0A-BC90-D4DFAA84E0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hóa đơn bán hàng" sheetId="1" r:id="rId1"/>
     <sheet name="Nguyên tắc ghép dữ liệu" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -450,15 +458,6 @@
     <t>Tỷ lệ chiết khấu (%)</t>
   </si>
   <si>
-    <t>Trường Tỷ lệ % trên doanh thu</t>
-  </si>
-  <si>
-    <t>Trường Tiền giảm 20% mức tỷ lệ</t>
-  </si>
-  <si>
-    <t>Trường Tiền giảm 20% mức tỷ lệ quy đổi</t>
-  </si>
-  <si>
     <t>Nhập Tiền giảm 20% mức tỷ lệ
 Tối đa 15 ký tự</t>
   </si>
@@ -652,9 +651,6 @@
     <t>HHDV 39</t>
   </si>
   <si>
-    <t>Trường Mặt hàng giảm</t>
-  </si>
-  <si>
     <t>Nhập là Mặt hàng giảm/Mặt hàng không giảm
 - Nhập 1: Mặt hàng giảm
 - Nhập 0 hoặc Để trống: Mặt hàng không giảm</t>
@@ -662,6 +658,18 @@
   <si>
     <t>Nhập Tỷ lệ % trên doanh thu.
 Lớn hơn 0</t>
+  </si>
+  <si>
+    <t>Mặt hàng giảm</t>
+  </si>
+  <si>
+    <t>Tỷ lệ % trên doanh thu</t>
+  </si>
+  <si>
+    <t>Tiền giảm 20% mức tỷ lệ</t>
+  </si>
+  <si>
+    <t>Tiền giảm 20% mức tỷ lệ quy đổi</t>
   </si>
 </sst>
 </file>
@@ -1368,7 +1376,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1383,7 +1391,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1423,28 +1431,28 @@
         <v>79</v>
       </c>
       <c r="E12" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="H12" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="I12" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="G12" s="29" t="s">
+      <c r="J12" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="K12" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="I12" s="29" t="s">
+      <c r="L12" s="29" t="s">
         <v>135</v>
-      </c>
-      <c r="J12" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="K12" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="L12" s="29" t="s">
-        <v>138</v>
       </c>
       <c r="M12" s="29" t="s">
         <v>77</v>
@@ -1453,36 +1461,36 @@
         <v>78</v>
       </c>
       <c r="O12" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="P12" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q12" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="R12" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="P12" s="29" t="s">
+      <c r="S12" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="Q12" s="29" t="s">
+      <c r="T12" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="R12" s="29" t="s">
+      <c r="U12" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="S12" s="29" t="s">
+      <c r="V12" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="T12" s="29" t="s">
+      <c r="W12" s="29" t="s">
         <v>144</v>
-      </c>
-      <c r="U12" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="V12" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="W12" s="29" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>0</v>
@@ -1590,8 +1598,8 @@
   </sheetPr>
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,7 +1675,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>4</v>
@@ -1681,7 +1689,7 @@
         <v>36</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>82</v>
@@ -1695,7 +1703,7 @@
         <v>36</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>12</v>
@@ -1709,7 +1717,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>2</v>
@@ -1723,7 +1731,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>3</v>
@@ -1737,7 +1745,7 @@
         <v>36</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>6</v>
@@ -1751,7 +1759,7 @@
         <v>36</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>5</v>
@@ -1765,7 +1773,7 @@
         <v>36</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>38</v>
@@ -1779,7 +1787,7 @@
         <v>36</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>39</v>
@@ -1793,7 +1801,7 @@
         <v>36</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>40</v>
@@ -1835,7 +1843,7 @@
         <v>37</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>88</v>
@@ -1849,7 +1857,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>20</v>
@@ -1863,7 +1871,7 @@
         <v>37</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>21</v>
@@ -1877,13 +1885,13 @@
         <v>37</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>120</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1891,7 +1899,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>22</v>
@@ -1905,7 +1913,7 @@
         <v>37</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>7</v>
@@ -1919,7 +1927,7 @@
         <v>37</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>8</v>
@@ -1933,7 +1941,7 @@
         <v>37</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>23</v>
@@ -1947,7 +1955,7 @@
         <v>37</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>9</v>
@@ -1961,7 +1969,7 @@
         <v>37</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>24</v>
@@ -1975,7 +1983,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>10</v>
@@ -1989,7 +1997,7 @@
         <v>37</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>15</v>
@@ -2003,7 +2011,7 @@
         <v>37</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>25</v>
@@ -2017,7 +2025,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>26</v>
@@ -2031,7 +2039,7 @@
         <v>37</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>27</v>
@@ -2045,7 +2053,7 @@
         <v>37</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>28</v>
@@ -2059,7 +2067,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>11</v>
@@ -2073,7 +2081,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>16</v>
@@ -2087,7 +2095,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>29</v>
@@ -2101,7 +2109,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>30</v>
@@ -2115,7 +2123,7 @@
         <v>37</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>31</v>
@@ -2129,7 +2137,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>32</v>
@@ -2143,7 +2151,7 @@
         <v>37</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>33</v>
@@ -2157,7 +2165,7 @@
         <v>37</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>34</v>
@@ -2171,7 +2179,7 @@
         <v>37</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>119</v>
@@ -2185,7 +2193,7 @@
         <v>37</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>118</v>
@@ -2199,7 +2207,7 @@
         <v>37</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>44</v>
@@ -2213,7 +2221,7 @@
         <v>37</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>45</v>
@@ -2227,7 +2235,7 @@
         <v>37</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>46</v>
@@ -2241,7 +2249,7 @@
         <v>37</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>47</v>
@@ -2255,7 +2263,7 @@
         <v>37</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>48</v>
@@ -2269,7 +2277,7 @@
         <v>37</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>49</v>
@@ -2283,7 +2291,7 @@
         <v>37</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>50</v>
@@ -2297,7 +2305,7 @@
         <v>37</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C54" s="13" t="s">
         <v>51</v>
@@ -2311,7 +2319,7 @@
         <v>37</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>52</v>
@@ -2325,7 +2333,7 @@
         <v>37</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C56" s="13" t="s">
         <v>53</v>
@@ -2339,13 +2347,13 @@
         <v>37</v>
       </c>
       <c r="B57" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="D57" s="11" t="s">
         <v>177</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2353,13 +2361,13 @@
         <v>37</v>
       </c>
       <c r="B58" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D58" s="11" t="s">
         <v>178</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2367,13 +2375,13 @@
         <v>37</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>123</v>
+        <v>181</v>
       </c>
       <c r="D59" s="34" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2381,13 +2389,13 @@
         <v>37</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>124</v>
+        <v>182</v>
       </c>
       <c r="D60" s="34" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update mau import excel hoa don
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
+++ b/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\Template\ImportHoaDon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66D6DC4-E25A-4C0A-BC90-D4DFAA84E0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7452F12F-B56D-4F78-848F-2074C93BA311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="184">
   <si>
     <t>Số thứ tự hóa đơn (*)</t>
   </si>
@@ -670,6 +670,9 @@
   </si>
   <si>
     <t>Tiền giảm 20% mức tỷ lệ quy đổi</t>
+  </si>
+  <si>
+    <t>HHDV 40</t>
   </si>
 </sst>
 </file>
@@ -2389,7 +2392,7 @@
         <v>37</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>152</v>
+        <v>183</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>182</v>

</xml_diff>

<commit_message>
Bug #1875: Điều chỉnh theo yêu cầu 01-07
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
+++ b/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\Template\ImportHoaDon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D8B0F2-88FC-4974-8FA2-2BA7B527B996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A825CC24-2200-444C-AA8C-F1DCE0D1CC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hóa đơn bán hàng" sheetId="1" r:id="rId1"/>
@@ -209,9 +209,6 @@
     <t>Nhập Ngày hóa đơn</t>
   </si>
   <si>
-    <t>Nhập Hình thức thanh toán</t>
-  </si>
-  <si>
     <t>Nhập Tài khoản ngân hàng</t>
   </si>
   <si>
@@ -222,19 +219,6 @@
   </si>
   <si>
     <t>Nhập Mã nhân viên bán hàng</t>
-  </si>
-  <si>
-    <t>Nhập Tên người mua hàng</t>
-  </si>
-  <si>
-    <t>Nhập Tên khách hàng</t>
-  </si>
-  <si>
-    <t>Nhập Địa chỉ khách hàng</t>
-  </si>
-  <si>
-    <t>Nhập Số điện thoại người nhận hóa đơn.
-Nếu nhiều số điện thoại thì mỗi số điện thoại cách nhau bởi dấu ";"</t>
   </si>
   <si>
     <t>Nhập Đơn vị tính</t>
@@ -268,13 +252,6 @@
   </si>
   <si>
     <t>Nhập Tỷ lệ chiết khấu</t>
-  </si>
-  <si>
-    <t>Nhập Email người nhận hóa đơn.
-Nếu nhiều Email thì mỗi Email cách nhau bởi dấu ";"</t>
-  </si>
-  <si>
-    <t>Nhập Mã hàng hóa, dịch vụ</t>
   </si>
   <si>
     <t>LOAITIEN</t>
@@ -435,11 +412,6 @@
 Tối đa 14 ký tự</t>
   </si>
   <si>
-    <t>Nhập Tên hàng hóa, dịch vụ
-Trường dữ liệu bắt buộc.
-Không để trống</t>
-  </si>
-  <si>
     <t>CHỈ DÙNG CHO LOẠI HÓA ĐƠN GIÁ TRỊ GIA TĂNG</t>
   </si>
   <si>
@@ -673,6 +645,48 @@
   </si>
   <si>
     <t>HHDV 40</t>
+  </si>
+  <si>
+    <t>Nhập Tên người mua hàng
+Tối đa 100 ký tự</t>
+  </si>
+  <si>
+    <t>Nhập Tên khách hàng
+Tối đa 400 ký tự</t>
+  </si>
+  <si>
+    <t>Nhập Địa chỉ khách hàng
+Tối đa 400 ký tự</t>
+  </si>
+  <si>
+    <t>Nhập Hình thức thanh toán
+Trường dữ liệu bắt buộc. Không để trống.
+Nhập 1: Tiền mặt
+Nhập 2: Chuyển khoản
+Nhập 3: Tiền mặt/Chuyển khoản
+Nhập 4: Đối trừ công nợ
+Nhập 5: Không thu tiền
+Nhập 6: Khác
+Hoặc nhập hình thức thanh toán tối đa 50 ký tự.</t>
+  </si>
+  <si>
+    <t>Nhập Email người nhận hóa đơn.
+Nếu nhiều Email thì mỗi Email cách nhau bởi dấu ";"
+Tối đa 50 ký tự</t>
+  </si>
+  <si>
+    <t>Nhập Số điện thoại người nhận hóa đơn.
+Nếu nhiều số điện thoại thì mỗi số điện thoại cách nhau bởi dấu ";"
+Tối đa 20 ký tự</t>
+  </si>
+  <si>
+    <t>Nhập Mã hàng hóa, dịch vụ
+Tối đa 50 ký tự</t>
+  </si>
+  <si>
+    <t>Nhập Tên hàng hóa, dịch vụ
+Trường dữ liệu bắt buộc.
+Không để trống, tối đa 400 ký tự</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1288,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1304,7 +1318,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1334,7 +1348,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1349,7 +1363,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1364,7 +1378,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1379,7 +1393,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1394,7 +1408,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1422,78 +1436,78 @@
     </row>
     <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E12" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="I12" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="J12" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="K12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="L12" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="N12" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="O12" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="P12" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="G12" s="29" t="s">
+      <c r="Q12" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="R12" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="I12" s="29" t="s">
+      <c r="S12" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="J12" s="29" t="s">
+      <c r="T12" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="K12" s="29" t="s">
+      <c r="U12" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="L12" s="29" t="s">
+      <c r="V12" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="M12" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="N12" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="O12" s="29" t="s">
+      <c r="W12" s="29" t="s">
         <v>136</v>
-      </c>
-      <c r="P12" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q12" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="R12" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="S12" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="T12" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="U12" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="V12" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="W12" s="29" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>0</v>
@@ -1535,7 +1549,7 @@
         <v>14</v>
       </c>
       <c r="O13" s="24" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="P13" s="24" t="s">
         <v>7</v>
@@ -1553,7 +1567,7 @@
         <v>15</v>
       </c>
       <c r="U13" s="26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="V13" s="26" t="s">
         <v>26</v>
@@ -1566,17 +1580,17 @@
   <dataValidations count="24">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập số thứ tự của hóa đơn._x000a_Lưu ý: Mỗi số thứ tự sẽ tương ứng với 1 hóa đơn_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống." sqref="B13:B1048576" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Ngày hóa đơn." sqref="D13:D1048576" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên người mua hàng" sqref="E13:E1048576" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên khách hàng" sqref="F13:F1048576" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Địa chỉ" sqref="G13:G1048576" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên người mua hàng_x000a_Tối đa 100 ký tự" sqref="E13:E1048576" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên khách hàng_x000a_Tối đa 400 ký tự" sqref="F13:F1048576" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Địa chỉ khách hàng_x000a_Tối đa 400 ký tự" sqref="G13:G1048576" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã số thuế_x000a_Tối đa 14 ký tự" sqref="H13:H1048576" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Hình thức thanh toán_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống._x000a_Nhập 1: Tiền mặt_x000a_Nhập 2: Chuyển khoản_x000a_Nhập 3: Tiền mặt/Chuyển khoản_x000a_Nhập 4: Đối trừ công nợ_x000a_Nhập 5: Không thu tiền_x000a_Nhập 6: Khác" sqref="I13:I1048576" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Email người nhận hóa đơn._x000a_Nếu nhiều Email thì mỗi Email cách nhau bởi dấu &quot;;&quot;" sqref="J13:J1048576" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Hình thức thanh toán_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống._x000a_Nhập 1: Tiền mặt_x000a_Nhập 2: Chuyển khoản_x000a_Nhập 3: Tiền mặt/Chuyển khoản_x000a_Nhập 4: Đối trừ công nợ_x000a_Nhập 5: Không thu tiền_x000a_Nhập 6: Khác_x000a_Hoặc nhập hình thức thanh toán tối đa 50 ký tự." sqref="I13:I1048576" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Email người nhận hóa đơn._x000a_Nếu nhiều Email thì mỗi Email cách nhau bởi dấu &quot;;&quot;_x000a_Tối đa 50 ký tự" sqref="J13:J1048576" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Số tài khoản ngân hàng" sqref="K13:K1048576" xr:uid="{00000000-0002-0000-0100-000008000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên ngân hàng" sqref="L13:L1048576" xr:uid="{00000000-0002-0000-0100-000009000000}"/>
     <dataValidation showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã loại tiền._x000a_Nếu để trống ngầm định là VND." sqref="M13:M1048576" xr:uid="{00000000-0002-0000-0100-00000A000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tỷ giá_x000a_Tối đa 15 ký tự" sqref="N13:N1048576" xr:uid="{00000000-0002-0000-0100-00000B000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên hàng hóa, dịch vụ._x000a_Trường dữ liệu bắt buộc._x000a_Không để trống" sqref="O13:O1048576" xr:uid="{00000000-0002-0000-0100-00000C000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên hàng hóa, dịch vụ_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống, tối đa 400 ký tự" sqref="O13:O1048576" xr:uid="{00000000-0002-0000-0100-00000C000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn vị tính." sqref="P13:P1048576" xr:uid="{00000000-0002-0000-0100-00000D000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền quy đổi_x000a_Tối đa 15 ký tự" sqref="T13:T1048576" xr:uid="{00000000-0002-0000-0100-00000E000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền_x000a_Tối đa 15 ký tự" sqref="S13:S1048576" xr:uid="{00000000-0002-0000-0100-00000F000000}"/>
@@ -1615,17 +1629,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1636,13 +1650,13 @@
         <v>35</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1650,7 +1664,7 @@
         <v>54</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>1</v>
@@ -1661,30 +1675,30 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>55</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>62</v>
+      <c r="D9" s="11" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1692,41 +1706,41 @@
         <v>36</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>64</v>
+      <c r="D12" s="11" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1734,55 +1748,55 @@
         <v>36</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D14" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>65</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1790,13 +1804,13 @@
         <v>36</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1804,13 +1818,13 @@
         <v>36</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>40</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1818,7 +1832,7 @@
         <v>41</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>13</v>
@@ -1832,7 +1846,7 @@
         <v>41</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>14</v>
@@ -1846,27 +1860,27 @@
         <v>37</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>76</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1874,13 +1888,13 @@
         <v>37</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>115</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -1888,13 +1902,13 @@
         <v>37</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1902,13 +1916,13 @@
         <v>37</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1916,13 +1930,13 @@
         <v>37</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1930,13 +1944,13 @@
         <v>37</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1944,13 +1958,13 @@
         <v>37</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1958,13 +1972,13 @@
         <v>37</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1972,13 +1986,13 @@
         <v>37</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1986,13 +2000,13 @@
         <v>37</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2000,13 +2014,13 @@
         <v>37</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2014,13 +2028,13 @@
         <v>37</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2028,13 +2042,13 @@
         <v>37</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2042,13 +2056,13 @@
         <v>37</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2056,13 +2070,13 @@
         <v>37</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>28</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2070,13 +2084,13 @@
         <v>37</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2084,13 +2098,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>16</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2098,13 +2112,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>29</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2112,13 +2126,13 @@
         <v>37</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2126,13 +2140,13 @@
         <v>37</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>31</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2140,13 +2154,13 @@
         <v>37</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2154,13 +2168,13 @@
         <v>37</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>33</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2168,13 +2182,13 @@
         <v>37</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>34</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2182,13 +2196,13 @@
         <v>37</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2196,13 +2210,13 @@
         <v>37</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2210,13 +2224,13 @@
         <v>37</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>44</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2224,13 +2238,13 @@
         <v>37</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>45</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2238,13 +2252,13 @@
         <v>37</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>46</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2252,13 +2266,13 @@
         <v>37</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>47</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2266,13 +2280,13 @@
         <v>37</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>48</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2280,13 +2294,13 @@
         <v>37</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>49</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2294,13 +2308,13 @@
         <v>37</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>50</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2308,13 +2322,13 @@
         <v>37</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C54" s="13" t="s">
         <v>51</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2322,13 +2336,13 @@
         <v>37</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>52</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2336,13 +2350,13 @@
         <v>37</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C56" s="13" t="s">
         <v>53</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2350,13 +2364,13 @@
         <v>37</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2364,13 +2378,13 @@
         <v>37</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2378,13 +2392,13 @@
         <v>37</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D59" s="34" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2392,13 +2406,13 @@
         <v>37</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D60" s="34" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
dieu chinh max length tenHang
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
+++ b/API/wwwroot/docs/Template/ImportHoaDon/Hoa_Don_Ban_Hang_Import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\Template\ImportHoaDon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBD49B7-9547-44B1-AB78-33FDF58378E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79E487D-D7BF-4293-AFE7-A79F630D96B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -681,12 +681,12 @@
 Tối đa 50 ký tự</t>
   </si>
   <si>
+    <t>- Các cột có dấu (*) là những cột bắt buộc</t>
+  </si>
+  <si>
     <t>Nhập Tên hàng hóa, dịch vụ
 Trường dữ liệu bắt buộc.
-Không để trống, tối đa 400 ký tự</t>
-  </si>
-  <si>
-    <t>- Các cột có dấu (*) là những cột bắt buộc</t>
+Không để trống, tối đa 500 ký tự</t>
   </si>
 </sst>
 </file>
@@ -1303,7 +1303,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1590,7 +1590,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên ngân hàng" sqref="L13:L1048576" xr:uid="{00000000-0002-0000-0100-000009000000}"/>
     <dataValidation showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Mã loại tiền._x000a_Nếu để trống ngầm định là VND." sqref="M13:M1048576" xr:uid="{00000000-0002-0000-0100-00000A000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tỷ giá_x000a_Tối đa 15 ký tự" sqref="N13:N1048576" xr:uid="{00000000-0002-0000-0100-00000B000000}"/>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên hàng hóa, dịch vụ_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống, tối đa 400 ký tự" sqref="O13:O1048576" xr:uid="{00000000-0002-0000-0100-00000C000000}"/>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Tên hàng hóa, dịch vụ_x000a_Trường dữ liệu bắt buộc._x000a_Không để trống, tối đa 500 ký tự" sqref="O13:O1048576" xr:uid="{00000000-0002-0000-0100-00000C000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Đơn vị tính." sqref="P13:P1048576" xr:uid="{00000000-0002-0000-0100-00000D000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền quy đổi_x000a_Tối đa 15 ký tự" sqref="T13:T1048576" xr:uid="{00000000-0002-0000-0100-00000E000000}"/>
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="HOADON-BACHKHOA" prompt="Nhập Thành tiền_x000a_Tối đa 15 ký tự" sqref="S13:S1048576" xr:uid="{00000000-0002-0000-0100-00000F000000}"/>
@@ -1894,7 +1894,7 @@
         <v>20</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">

</xml_diff>